<commit_message>
separando as funcoes de formacacao de data e hora
</commit_message>
<xml_diff>
--- a/assets/forerunner_255s.xlsx
+++ b/assets/forerunner_255s.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Q+nbzI+dRUyhxZOY5hKZT9NcAlcFCZHLVeMJMBdHgpw="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="udYd2N88BqaB0T9qnm17R4XZAG4dNn+1yXNzoQpQH6w="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="30">
   <si>
     <t>data</t>
   </si>
@@ -103,15 +103,6 @@
   </si>
   <si>
     <t>14:45</t>
-  </si>
-  <si>
-    <t>20:26</t>
-  </si>
-  <si>
-    <t>20:35</t>
-  </si>
-  <si>
-    <t>21:17</t>
   </si>
   <si>
     <t>21:23</t>
@@ -1348,7 +1339,7 @@
         <v>29</v>
       </c>
       <c r="C56" s="3">
-        <v>2489.0</v>
+        <v>2476.33</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>6</v>
@@ -1374,74 +1365,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="2">
-        <v>45201.0</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="3">
-        <v>2589.0</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="2">
-        <v>45201.0</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="3">
-        <v>2476.33</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="2">
-        <v>45201.0</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="3">
-        <v>2476.33</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="2">
-        <v>45201.0</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="3">
-        <v>2589.0</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
@@ -2377,10 +2304,6 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>